<commit_message>
Added facility filter method.
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log_2023.xlsx
+++ b/DTT-Assessment-Hour-Log_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\catering_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFAD921-F174-4D9A-BF31-C920818216EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C70E9E-A371-48DE-859F-7BE0BBCC0058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <r>
       <rPr>
@@ -75,9 +75,6 @@
     <t>Bonus</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Total amount of hours</t>
   </si>
   <si>
@@ -109,6 +106,24 @@
   </si>
   <si>
     <t>Implemented feature to create a facility.</t>
+  </si>
+  <si>
+    <t>Created method for updating facility</t>
+  </si>
+  <si>
+    <t>Created method for deleting facilities</t>
+  </si>
+  <si>
+    <t>Impleted a method which allows the deletion of a facility by its name.</t>
+  </si>
+  <si>
+    <t>Impleted method which allows you to edit a facility and it tags.</t>
+  </si>
+  <si>
+    <t>Created method to filter facilities</t>
+  </si>
+  <si>
+    <t>Impleted method so you can get faciliteis by their name, location and tags.</t>
   </si>
 </sst>
 </file>
@@ -339,12 +354,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -377,6 +386,12 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -812,7 +827,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.53515625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -825,327 +840,349 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>45066</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8">
+      <c r="E4" s="9"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="7">
+        <v>45066</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7">
+        <v>45069</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="9">
-        <v>45066</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="8">
+      <c r="C7" s="7">
+        <v>45069</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>45069</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>45069</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6">
         <v>0.5</v>
       </c>
-      <c r="C5" s="9">
-        <v>45066</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8">
-        <v>2</v>
-      </c>
-      <c r="C6" s="9">
+      <c r="C10" s="7">
         <v>45069</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="D10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7">
+        <v>45069</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" s="9">
-        <v>45069</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9">
-        <v>45069</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="16">
+      <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>3.5</v>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="6"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="6"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="20"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>